<commit_message>
parte plao de projeto
</commit_message>
<xml_diff>
--- a/Sistema/000-Requisitos/PBL-Product Backlog.xlsx
+++ b/Sistema/000-Requisitos/PBL-Product Backlog.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t xml:space="preserve">PRODUCT BACKLOG</t>
+    <t xml:space="preserve">PRODUCT BACKLOG – AJUDE MAIS</t>
   </si>
   <si>
     <t xml:space="preserve">Nome / Descrição</t>
@@ -288,19 +288,19 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1821862348178"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7975708502024"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0971659919028"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>

<commit_message>
atualização de plano de projeto
</commit_message>
<xml_diff>
--- a/Sistema/000-Requisitos/PBL-Product Backlog.xlsx
+++ b/Sistema/000-Requisitos/PBL-Product Backlog.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Ajude Mais\Sistema\000-Requisitos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,115 +28,110 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
-    <t xml:space="preserve">PRODUCT BACKLOG – AJUDE MAIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nome / Descrição</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prioridade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Módulo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamanho em Story Points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iteração Prevista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assig-ned To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horas Estimadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horas Trabalhadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMBOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de instituições de caridade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de categorias de itens de doação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de doadores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizar doação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOBILE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de mensageiros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizar coleta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrar entrega de coleta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de campanhas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de metas de campanha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acompanhamento de doações</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acompanhamento de coletas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notificação de doações</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notificação de campanhas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizar entrega de doação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartilhar doação e campanha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de conta de usuário</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de “super usuários”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerar relatórios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gamificação de doadores e mensageiros</t>
+    <t>PRODUCT BACKLOG – AJUDE MAIS</t>
+  </si>
+  <si>
+    <t>Nome / Descrição</t>
+  </si>
+  <si>
+    <t>Prioridade</t>
+  </si>
+  <si>
+    <t>Módulo</t>
+  </si>
+  <si>
+    <t>Tamanho em Story Points</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Iteração Prevista</t>
+  </si>
+  <si>
+    <t>Assig-ned To</t>
+  </si>
+  <si>
+    <t>Horas Estimadas</t>
+  </si>
+  <si>
+    <t>Horas Trabalhadas</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>AMBOS</t>
+  </si>
+  <si>
+    <t>Gerenciamento de instituições de caridade</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>Gerenciamento de categorias de itens de doação</t>
+  </si>
+  <si>
+    <t>Gerenciamento de doadores</t>
+  </si>
+  <si>
+    <t>Realizar doação</t>
+  </si>
+  <si>
+    <t>MOBILE</t>
+  </si>
+  <si>
+    <t>Gerenciamento de mensageiros</t>
+  </si>
+  <si>
+    <t>Realizar coleta</t>
+  </si>
+  <si>
+    <t>Registrar entrega de coleta</t>
+  </si>
+  <si>
+    <t>Gerenciamento de campanhas</t>
+  </si>
+  <si>
+    <t>Gerenciamento de metas de campanha</t>
+  </si>
+  <si>
+    <t>Acompanhamento de doações</t>
+  </si>
+  <si>
+    <t>Acompanhamento de coletas</t>
+  </si>
+  <si>
+    <t>Notificação de doações</t>
+  </si>
+  <si>
+    <t>Notificação de campanhas</t>
+  </si>
+  <si>
+    <t>Realizar entrega de doação</t>
+  </si>
+  <si>
+    <t>Compartilhar doação e campanha</t>
+  </si>
+  <si>
+    <t>Gerenciamento de conta de usuário</t>
+  </si>
+  <si>
+    <t>Gerenciamento de “super usuários”</t>
+  </si>
+  <si>
+    <t>Gerar relatórios</t>
+  </si>
+  <si>
+    <t>Gamificação de doadores e mensageiros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -142,20 +141,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -163,15 +155,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -191,7 +175,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -226,128 +210,73 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -406,50 +335,324 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="45.42578125" style="2"/>
+    <col min="2" max="2" width="10.5703125"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="20"/>
+    <col min="5" max="5" width="8.5703125"/>
+    <col min="6" max="6" width="11.7109375"/>
+    <col min="7" max="7" width="10.85546875"/>
+    <col min="8" max="8" width="16.42578125"/>
+    <col min="9" max="9" width="13.42578125"/>
+    <col min="10" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -478,252 +681,252 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D3" s="8">
         <v>5</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="8">
         <v>1</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="8">
         <v>2</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="8">
         <v>1</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="8">
         <v>1</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="7">
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="8">
         <v>2</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8" t="n">
+      <c r="D7" s="8">
         <v>13</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="8">
         <v>2</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="7" t="n">
+      <c r="B8" s="7">
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="n">
+      <c r="D8" s="8">
         <v>5</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="8">
         <v>3</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="7">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="8" t="n">
+      <c r="D9" s="8">
         <v>20</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="8">
         <v>3</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="7">
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="8" t="n">
+      <c r="D10" s="8">
         <v>3</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="8" t="n">
+      <c r="F10" s="8">
         <v>4</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="7">
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="8" t="n">
+      <c r="D11" s="8">
         <v>20</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="8" t="n">
+      <c r="F11" s="8">
         <v>5</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="7">
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="8" t="n">
+      <c r="D12" s="8">
         <v>2</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="8">
         <v>5</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="7">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="n">
+      <c r="D13" s="8">
         <v>2</v>
       </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="8" t="n">
+      <c r="F13" s="8">
         <v>5</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="7">
         <v>12</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="11" t="n">
+      <c r="D14" s="11">
         <v>2</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="13" t="n">
+      <c r="F14" s="13">
         <v>6</v>
       </c>
       <c r="G14" s="13"/>
@@ -731,21 +934,21 @@
       <c r="I14" s="13"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="7">
         <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="11" t="n">
+      <c r="D15" s="11">
         <v>13</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="13" t="n">
+      <c r="F15" s="13">
         <v>6</v>
       </c>
       <c r="G15" s="13"/>
@@ -753,17 +956,17 @@
       <c r="I15" s="13"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="7">
         <v>14</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="11" t="n">
+      <c r="D16" s="11">
         <v>13</v>
       </c>
       <c r="E16" s="12"/>
@@ -773,17 +976,17 @@
       <c r="I16" s="13"/>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="7">
         <v>15</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="11" t="n">
+      <c r="D17" s="11">
         <v>3</v>
       </c>
       <c r="E17" s="12"/>
@@ -793,17 +996,17 @@
       <c r="I17" s="13"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="7">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="11" t="n">
+      <c r="D18" s="11">
         <v>5</v>
       </c>
       <c r="E18" s="12"/>
@@ -813,17 +1016,17 @@
       <c r="I18" s="13"/>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="7" t="n">
+      <c r="B19" s="7">
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="11" t="n">
+      <c r="D19" s="11">
         <v>8</v>
       </c>
       <c r="E19" s="12"/>
@@ -833,17 +1036,17 @@
       <c r="I19" s="13"/>
       <c r="K19" s="14"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="7">
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="11" t="n">
+      <c r="D20" s="11">
         <v>5</v>
       </c>
       <c r="E20" s="12"/>
@@ -853,17 +1056,17 @@
       <c r="I20" s="13"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="7">
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="11" t="n">
+      <c r="D21" s="11">
         <v>5</v>
       </c>
       <c r="E21" s="12"/>
@@ -873,17 +1076,17 @@
       <c r="I21" s="13"/>
       <c r="K21" s="14"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="7" t="n">
+      <c r="B22" s="7">
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="11" t="n">
+      <c r="D22" s="11">
         <v>5</v>
       </c>
       <c r="E22" s="12"/>
@@ -892,7 +1095,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -903,7 +1106,7 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -914,7 +1117,7 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -925,7 +1128,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -936,7 +1139,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -947,7 +1150,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -958,7 +1161,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -973,64 +1176,39 @@
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
recuperando donativos ordenados pela data de criação
</commit_message>
<xml_diff>
--- a/Sistema/000-Requisitos/PBL-Product Backlog.xlsx
+++ b/Sistema/000-Requisitos/PBL-Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t xml:space="preserve">PRODUCT BACKLOG – AJUDE MAIS</t>
   </si>
@@ -63,6 +63,9 @@
     <t xml:space="preserve">Pronto</t>
   </si>
   <si>
+    <t xml:space="preserve">~51</t>
+  </si>
+  <si>
     <t xml:space="preserve">~ 60</t>
   </si>
   <si>
@@ -72,7 +75,7 @@
     <t xml:space="preserve">WEB</t>
   </si>
   <si>
-    <t xml:space="preserve">30.5</t>
+    <t xml:space="preserve">~30.5</t>
   </si>
   <si>
     <t xml:space="preserve">~28</t>
@@ -81,7 +84,7 @@
     <t xml:space="preserve">Gerenciamento de categorias de itens de doação</t>
   </si>
   <si>
-    <t xml:space="preserve">20.5</t>
+    <t xml:space="preserve">~20.5</t>
   </si>
   <si>
     <t xml:space="preserve">~15</t>
@@ -108,18 +111,15 @@
     <t xml:space="preserve">Realizar doação avulsa </t>
   </si>
   <si>
-    <t xml:space="preserve">Implementação de notificação do lado do servidor</t>
+    <t xml:space="preserve">Gerenciamento de campanhas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de notificação</t>
   </si>
   <si>
     <t xml:space="preserve">WS</t>
   </si>
   <si>
-    <t xml:space="preserve">2.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerenciamento de campanhas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Realizar coleta</t>
   </si>
   <si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gerenciamento de metas de campanha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acompanhamento de doações</t>
   </si>
   <si>
     <t xml:space="preserve">Acompanhamento de coletas</t>
@@ -297,7 +294,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -350,20 +347,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -479,7 +468,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
@@ -487,10 +476,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.9878542510121"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.9271255060729"/>
@@ -561,22 +550,22 @@
         <v>1</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="6" t="n">
-        <v>51</v>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>5</v>
@@ -589,21 +578,21 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>2</v>
@@ -616,21 +605,21 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>3</v>
@@ -643,21 +632,21 @@
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>6</v>
@@ -670,62 +659,62 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="11" t="n">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="B9" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="D10" s="12" t="n">
         <v>8</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="12" t="n">
-        <v>5</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -777,7 +766,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="12" t="n">
         <v>3</v>
@@ -796,7 +785,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="12" t="n">
         <v>3</v>
@@ -807,12 +796,12 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="11" t="n">
-        <v>13</v>
+      <c r="B15" s="14" t="n">
+        <v>14</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>11</v>
@@ -820,268 +809,250 @@
       <c r="D15" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="11" t="n">
-        <v>14</v>
+      <c r="B16" s="14" t="n">
+        <v>15</v>
       </c>
       <c r="C16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="14" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="14" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="14" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="14" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="17" t="n">
-        <v>3</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="11" t="n">
-        <v>15</v>
-      </c>
-      <c r="C17" s="14" t="s">
+      <c r="D20" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="14" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="14" t="n">
         <v>22</v>
       </c>
-      <c r="D17" s="17" t="n">
-        <v>13</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="11" t="n">
-        <v>16</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="17" t="n">
-        <v>13</v>
-      </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="11" t="n">
-        <v>17</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="17" t="n">
-        <v>3</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="K19" s="20"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="11" t="n">
-        <v>18</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="17" t="n">
+      <c r="C23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="11" t="n">
-        <v>19</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="17" t="n">
-        <v>8</v>
-      </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="11" t="n">
-        <v>20</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="K22" s="20"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="11" t="n">
-        <v>21</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="K23" s="20"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="11" t="n">
-        <v>22</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="E24" s="18"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="22"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-    </row>
+      <c r="A30" s="22"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
@@ -1114,8 +1085,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
-        <v>46</v>
+      <c r="A1" s="23" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>